<commit_message>
Microbiome app staerted on 17th February
</commit_message>
<xml_diff>
--- a/WBFFQ/DB and Documents/WBFFQ.xlsx
+++ b/WBFFQ/DB and Documents/WBFFQ.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="382">
   <si>
     <t>Qdesceng</t>
   </si>
@@ -257,9 +257,6 @@
   </si>
   <si>
     <t>c606</t>
-  </si>
-  <si>
-    <t>c607</t>
   </si>
   <si>
     <t>c607a</t>
@@ -2247,7 +2244,7 @@
       <pane xSplit="5" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomRight" activeCell="U2" sqref="U2:U31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="29.25" customHeight="1"/>
@@ -2446,11 +2443,11 @@
         <v>35</v>
       </c>
       <c r="F2" s="60" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G2" s="61"/>
       <c r="H2" s="58" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I2" s="58"/>
       <c r="J2" s="62"/>
@@ -2480,7 +2477,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="58" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C3" s="58" t="s">
         <v>26</v>
@@ -2492,7 +2489,7 @@
         <v>1.2</v>
       </c>
       <c r="F3" s="60" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G3" s="61"/>
       <c r="H3" s="58" t="s">
@@ -2538,7 +2535,7 @@
         <v>1.3</v>
       </c>
       <c r="F4" s="68" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G4" s="66"/>
       <c r="H4" s="65" t="s">
@@ -2588,7 +2585,7 @@
       </c>
       <c r="G5" s="66"/>
       <c r="H5" s="65" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="I5" s="58"/>
       <c r="J5" s="62"/>
@@ -2618,7 +2615,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="65" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C6" s="58" t="s">
         <v>26</v>
@@ -2630,11 +2627,11 @@
         <v>1.8</v>
       </c>
       <c r="F6" s="68" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G6" s="66"/>
       <c r="H6" s="65" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="I6" s="58"/>
       <c r="L6" s="63"/>
@@ -2662,7 +2659,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="65" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C7" s="58" t="s">
         <v>23</v>
@@ -2674,11 +2671,11 @@
         <v>1.9</v>
       </c>
       <c r="F7" s="68" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G7" s="66"/>
       <c r="H7" s="65" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="I7" s="58"/>
       <c r="L7" s="63"/>
@@ -2706,10 +2703,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="65" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C8" s="58" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D8" s="58" t="s">
         <v>27</v>
@@ -2718,7 +2715,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="F8" s="68" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G8" s="66"/>
       <c r="H8" s="65" t="s">
@@ -2805,10 +2802,10 @@
         <v>29</v>
       </c>
       <c r="E10" s="75" t="s">
+        <v>96</v>
+      </c>
+      <c r="F10" s="76" t="s">
         <v>97</v>
-      </c>
-      <c r="F10" s="76" t="s">
-        <v>98</v>
       </c>
       <c r="G10" s="72"/>
       <c r="H10" s="58" t="s">
@@ -2851,7 +2848,7 @@
         <v>29</v>
       </c>
       <c r="E11" s="75" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F11" s="76" t="s">
         <v>38</v>
@@ -2943,10 +2940,10 @@
         <v>27</v>
       </c>
       <c r="E13" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="F13" s="44" t="s">
         <v>108</v>
-      </c>
-      <c r="F13" s="44" t="s">
-        <v>109</v>
       </c>
       <c r="G13" s="45"/>
       <c r="H13" s="58" t="s">
@@ -3127,7 +3124,7 @@
         <v>27</v>
       </c>
       <c r="E17" s="43" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F17" s="52" t="s">
         <v>45</v>
@@ -3176,11 +3173,11 @@
         <v>46</v>
       </c>
       <c r="F18" s="54" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G18" s="45"/>
       <c r="H18" s="42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I18" s="42"/>
       <c r="J18" s="45"/>
@@ -3210,7 +3207,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C19" s="42" t="s">
         <v>25</v>
@@ -3256,7 +3253,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="42" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C20" s="42" t="s">
         <v>23</v>
@@ -3265,10 +3262,10 @@
         <v>27</v>
       </c>
       <c r="E20" s="77" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F20" s="56" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G20" s="45"/>
       <c r="H20" s="58" t="s">
@@ -3311,14 +3308,14 @@
         <v>29</v>
       </c>
       <c r="E21" s="49" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F21" s="56" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G21" s="45"/>
       <c r="H21" s="58" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I21" s="42"/>
       <c r="J21" s="45"/>
@@ -3348,7 +3345,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C22" s="42" t="s">
         <v>30</v>
@@ -3403,14 +3400,14 @@
         <v>27</v>
       </c>
       <c r="E23" s="49" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F23" s="55" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G23" s="45"/>
       <c r="H23" s="58" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I23" s="42"/>
       <c r="J23" s="45"/>
@@ -3440,10 +3437,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C24" s="42" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D24" s="42" t="s">
         <v>27</v>
@@ -3456,7 +3453,7 @@
       </c>
       <c r="G24" s="45"/>
       <c r="H24" s="58" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I24" s="42"/>
       <c r="J24" s="45"/>
@@ -3486,7 +3483,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="42" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C25" s="42" t="s">
         <v>25</v>
@@ -3495,10 +3492,10 @@
         <v>27</v>
       </c>
       <c r="E25" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="F25" s="55" t="s">
         <v>99</v>
-      </c>
-      <c r="F25" s="55" t="s">
-        <v>100</v>
       </c>
       <c r="G25" s="45"/>
       <c r="H25" s="58" t="s">
@@ -3541,14 +3538,14 @@
         <v>63</v>
       </c>
       <c r="E26" s="49" t="s">
+        <v>117</v>
+      </c>
+      <c r="F26" s="55" t="s">
         <v>118</v>
-      </c>
-      <c r="F26" s="55" t="s">
-        <v>119</v>
       </c>
       <c r="G26" s="45"/>
       <c r="H26" s="58" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I26" s="42"/>
       <c r="J26" s="45"/>
@@ -3578,7 +3575,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C27" s="42" t="s">
         <v>23</v>
@@ -3587,7 +3584,7 @@
         <v>27</v>
       </c>
       <c r="E27" s="49" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F27" s="51" t="s">
         <v>53</v>
@@ -3633,14 +3630,14 @@
         <v>63</v>
       </c>
       <c r="E28" s="49" t="s">
+        <v>113</v>
+      </c>
+      <c r="F28" s="42" t="s">
         <v>114</v>
-      </c>
-      <c r="F28" s="42" t="s">
-        <v>115</v>
       </c>
       <c r="G28" s="45"/>
       <c r="H28" s="58" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I28" s="42"/>
       <c r="J28" s="45"/>
@@ -3670,7 +3667,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C29" s="42" t="s">
         <v>30</v>
@@ -3686,7 +3683,7 @@
       </c>
       <c r="G29" s="45"/>
       <c r="H29" s="58" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I29" s="42"/>
       <c r="J29" s="45"/>
@@ -3716,7 +3713,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="42" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C30" s="42" t="s">
         <v>24</v>
@@ -3725,14 +3722,14 @@
         <v>29</v>
       </c>
       <c r="E30" s="49" t="s">
+        <v>93</v>
+      </c>
+      <c r="F30" s="42" t="s">
         <v>94</v>
-      </c>
-      <c r="F30" s="42" t="s">
-        <v>95</v>
       </c>
       <c r="G30" s="45"/>
       <c r="H30" s="42" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I30" s="42"/>
       <c r="J30" s="45"/>
@@ -3762,19 +3759,19 @@
         <v>30</v>
       </c>
       <c r="B31" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="C31" s="57" t="s">
         <v>121</v>
       </c>
-      <c r="C31" s="57" t="s">
+      <c r="D31" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="D31" s="42" t="s">
+      <c r="E31" s="49" t="s">
         <v>123</v>
       </c>
-      <c r="E31" s="49" t="s">
+      <c r="F31" s="51" t="s">
         <v>124</v>
-      </c>
-      <c r="F31" s="51" t="s">
-        <v>125</v>
       </c>
       <c r="G31" s="45"/>
       <c r="H31" s="42" t="s">
@@ -4444,8 +4441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H140"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A139"/>
+    <sheetView topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4459,23 +4456,23 @@
         <v>19</v>
       </c>
       <c r="B1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="81" t="s">
         <v>126</v>
       </c>
-      <c r="C1" s="81" t="s">
+      <c r="D1" s="79" t="s">
         <v>127</v>
       </c>
-      <c r="D1" s="79" t="s">
+      <c r="E1" s="80" t="s">
         <v>128</v>
       </c>
-      <c r="E1" s="80" t="s">
+      <c r="F1" s="80" t="s">
         <v>129</v>
-      </c>
-      <c r="F1" s="80" t="s">
-        <v>130</v>
       </c>
       <c r="G1" s="80"/>
       <c r="H1" s="80" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -4486,7 +4483,7 @@
         <v>67</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D2" s="82">
         <v>0</v>
@@ -4507,7 +4504,7 @@
         <v>67</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D3" s="82">
         <v>1</v>
@@ -4528,7 +4525,7 @@
         <v>67</v>
       </c>
       <c r="C4" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D4" s="82">
         <v>2</v>
@@ -4549,7 +4546,7 @@
         <v>67</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D5" s="82">
         <v>3</v>
@@ -4570,7 +4567,7 @@
         <v>67</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D6" s="82">
         <v>4</v>
@@ -4591,7 +4588,7 @@
         <v>67</v>
       </c>
       <c r="C7" s="34" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D7" s="82">
         <v>5</v>
@@ -4612,7 +4609,7 @@
         <v>67</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D8" s="82">
         <v>6</v>
@@ -4633,7 +4630,7 @@
         <v>67</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D9" s="82">
         <v>7</v>
@@ -4654,7 +4651,7 @@
         <v>67</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D10" s="82">
         <v>8</v>
@@ -4675,7 +4672,7 @@
         <v>67</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D11" s="82">
         <v>9</v>
@@ -4696,7 +4693,7 @@
         <v>67</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D12" s="82">
         <v>10</v>
@@ -4717,7 +4714,7 @@
         <v>67</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D13" s="82">
         <v>11</v>
@@ -4738,7 +4735,7 @@
         <v>67</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D14" s="82">
         <v>12</v>
@@ -4759,7 +4756,7 @@
         <v>67</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D15" s="82">
         <v>13</v>
@@ -4780,7 +4777,7 @@
         <v>67</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D16" s="82">
         <v>14</v>
@@ -4801,7 +4798,7 @@
         <v>67</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D17" s="82">
         <v>15</v>
@@ -4822,7 +4819,7 @@
         <v>67</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D18" s="82">
         <v>16</v>
@@ -4843,7 +4840,7 @@
         <v>67</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D19" s="82">
         <v>17</v>
@@ -4864,10 +4861,10 @@
         <v>67</v>
       </c>
       <c r="C20" s="34" t="s">
+        <v>149</v>
+      </c>
+      <c r="D20" s="82" t="s">
         <v>150</v>
-      </c>
-      <c r="D20" s="82" t="s">
-        <v>151</v>
       </c>
       <c r="E20">
         <v>88</v>
@@ -4885,10 +4882,10 @@
         <v>67</v>
       </c>
       <c r="C21" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="D21" s="82" t="s">
         <v>152</v>
-      </c>
-      <c r="D21" s="82" t="s">
-        <v>153</v>
       </c>
       <c r="E21">
         <v>99</v>
@@ -4906,10 +4903,10 @@
         <v>69</v>
       </c>
       <c r="C22" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="D22" s="82" t="s">
         <v>154</v>
-      </c>
-      <c r="D22" s="82" t="s">
-        <v>155</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -4930,10 +4927,10 @@
         <v>69</v>
       </c>
       <c r="C23" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="D23" s="82" t="s">
         <v>156</v>
-      </c>
-      <c r="D23" s="82" t="s">
-        <v>157</v>
       </c>
       <c r="E23">
         <v>2</v>
@@ -4951,10 +4948,10 @@
         <v>70</v>
       </c>
       <c r="C24" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="D24" s="82" t="s">
         <v>154</v>
-      </c>
-      <c r="D24" s="82" t="s">
-        <v>155</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -4972,10 +4969,10 @@
         <v>70</v>
       </c>
       <c r="C25" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="D25" s="82" t="s">
         <v>156</v>
-      </c>
-      <c r="D25" s="82" t="s">
-        <v>157</v>
       </c>
       <c r="E25">
         <v>2</v>
@@ -4996,10 +4993,10 @@
         <v>71</v>
       </c>
       <c r="C26" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="D26" s="82" t="s">
         <v>158</v>
-      </c>
-      <c r="D26" s="82" t="s">
-        <v>159</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -5017,10 +5014,10 @@
         <v>71</v>
       </c>
       <c r="C27" s="34" t="s">
+        <v>159</v>
+      </c>
+      <c r="D27" s="82" t="s">
         <v>160</v>
-      </c>
-      <c r="D27" s="82" t="s">
-        <v>161</v>
       </c>
       <c r="E27">
         <v>2</v>
@@ -5038,10 +5035,10 @@
         <v>71</v>
       </c>
       <c r="C28" s="34" t="s">
+        <v>161</v>
+      </c>
+      <c r="D28" s="82" t="s">
         <v>162</v>
-      </c>
-      <c r="D28" s="82" t="s">
-        <v>163</v>
       </c>
       <c r="E28">
         <v>3</v>
@@ -5059,10 +5056,10 @@
         <v>71</v>
       </c>
       <c r="C29" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="D29" s="82" t="s">
         <v>164</v>
-      </c>
-      <c r="D29" s="82" t="s">
-        <v>165</v>
       </c>
       <c r="E29">
         <v>4</v>
@@ -5104,10 +5101,10 @@
         <v>73</v>
       </c>
       <c r="C31" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="D31" s="82" t="s">
         <v>166</v>
-      </c>
-      <c r="D31" s="82" t="s">
-        <v>167</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -5125,10 +5122,10 @@
         <v>73</v>
       </c>
       <c r="C32" s="34" t="s">
+        <v>167</v>
+      </c>
+      <c r="D32" s="82" t="s">
         <v>168</v>
-      </c>
-      <c r="D32" s="82" t="s">
-        <v>169</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -5146,10 +5143,10 @@
         <v>73</v>
       </c>
       <c r="C33" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="D33" s="82" t="s">
         <v>170</v>
-      </c>
-      <c r="D33" s="82" t="s">
-        <v>171</v>
       </c>
       <c r="E33">
         <v>2</v>
@@ -5167,10 +5164,10 @@
         <v>73</v>
       </c>
       <c r="C34" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="D34" s="82" t="s">
         <v>172</v>
-      </c>
-      <c r="D34" s="82" t="s">
-        <v>173</v>
       </c>
       <c r="E34">
         <v>3</v>
@@ -5188,16 +5185,16 @@
         <v>73</v>
       </c>
       <c r="C35" s="34" t="s">
+        <v>173</v>
+      </c>
+      <c r="D35" s="82" t="s">
         <v>174</v>
-      </c>
-      <c r="D35" s="82" t="s">
-        <v>175</v>
       </c>
       <c r="E35">
         <v>88</v>
       </c>
       <c r="F35" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H35" s="35" t="str">
         <f t="shared" si="0"/>
@@ -5212,10 +5209,10 @@
         <v>73</v>
       </c>
       <c r="C36" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="D36" s="82" t="s">
         <v>176</v>
-      </c>
-      <c r="D36" s="82" t="s">
-        <v>177</v>
       </c>
       <c r="E36">
         <v>99</v>
@@ -5233,10 +5230,10 @@
         <v>74</v>
       </c>
       <c r="C37" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="D37" s="82" t="s">
         <v>154</v>
-      </c>
-      <c r="D37" s="82" t="s">
-        <v>155</v>
       </c>
       <c r="E37">
         <v>1</v>
@@ -5254,10 +5251,10 @@
         <v>74</v>
       </c>
       <c r="C38" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="D38" s="82" t="s">
         <v>156</v>
-      </c>
-      <c r="D38" s="82" t="s">
-        <v>157</v>
       </c>
       <c r="E38">
         <v>2</v>
@@ -5275,20 +5272,20 @@
         <v>75</v>
       </c>
       <c r="C39" s="34" t="s">
+        <v>177</v>
+      </c>
+      <c r="D39" s="82" t="s">
         <v>178</v>
-      </c>
-      <c r="D39" s="82" t="s">
-        <v>179</v>
       </c>
       <c r="E39">
         <v>1</v>
       </c>
-      <c r="F39" t="s">
-        <v>77</v>
+      <c r="F39" s="35" t="s">
+        <v>79</v>
       </c>
       <c r="H39" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('38','c605', 'Still, breastfeeding','GL‡bv ey‡Ki `ya cvb K‡i','1','c607');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('38','c605', 'Still, breastfeeding','GL‡bv ey‡Ki `ya cvb K‡i','1','c607c');</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="27">
@@ -5299,10 +5296,10 @@
         <v>75</v>
       </c>
       <c r="C40" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="D40" s="82" t="s">
         <v>180</v>
-      </c>
-      <c r="D40" s="82" t="s">
-        <v>181</v>
       </c>
       <c r="E40">
         <v>2</v>
@@ -5317,13 +5314,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C41" s="34" t="s">
+        <v>181</v>
+      </c>
+      <c r="D41" s="82" t="s">
         <v>182</v>
-      </c>
-      <c r="D41" s="82" t="s">
-        <v>183</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -5338,13 +5335,13 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C42" s="34" t="s">
+        <v>183</v>
+      </c>
+      <c r="D42" s="82" t="s">
         <v>184</v>
-      </c>
-      <c r="D42" s="82" t="s">
-        <v>185</v>
       </c>
       <c r="E42">
         <v>2</v>
@@ -5359,13 +5356,13 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C43" s="34" t="s">
+        <v>185</v>
+      </c>
+      <c r="D43" s="82" t="s">
         <v>186</v>
-      </c>
-      <c r="D43" s="82" t="s">
-        <v>187</v>
       </c>
       <c r="E43">
         <v>3</v>
@@ -5380,13 +5377,13 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C44" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="D44" s="82" t="s">
         <v>188</v>
-      </c>
-      <c r="D44" s="82" t="s">
-        <v>189</v>
       </c>
       <c r="E44">
         <v>4</v>
@@ -5401,19 +5398,19 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C45" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="D45" s="82" t="s">
         <v>190</v>
-      </c>
-      <c r="D45" s="82" t="s">
-        <v>191</v>
       </c>
       <c r="E45">
         <v>5</v>
       </c>
       <c r="F45" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H45" s="35" t="str">
         <f t="shared" si="0"/>
@@ -5425,13 +5422,13 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C46" s="34" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D46" s="82" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E46">
         <v>6</v>
@@ -5446,10 +5443,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C47" s="34" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D47" s="82" t="s">
         <v>56</v>
@@ -5458,7 +5455,7 @@
         <v>77</v>
       </c>
       <c r="F47" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H47" s="35" t="str">
         <f t="shared" si="0"/>
@@ -5470,19 +5467,19 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C48" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="D48" s="82" t="s">
         <v>154</v>
-      </c>
-      <c r="D48" s="82" t="s">
-        <v>155</v>
       </c>
       <c r="E48">
         <v>1</v>
       </c>
       <c r="F48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H48" s="35" t="str">
         <f t="shared" si="0"/>
@@ -5494,13 +5491,13 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C49" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="D49" s="82" t="s">
         <v>156</v>
-      </c>
-      <c r="D49" s="82" t="s">
-        <v>157</v>
       </c>
       <c r="E49">
         <v>2</v>
@@ -5518,13 +5515,13 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C50" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="D50" s="82" t="s">
         <v>176</v>
-      </c>
-      <c r="D50" s="82" t="s">
-        <v>177</v>
       </c>
       <c r="E50">
         <v>99</v>
@@ -5542,13 +5539,13 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
+        <v>193</v>
+      </c>
+      <c r="C51" s="34" t="s">
         <v>194</v>
       </c>
-      <c r="C51" s="34" t="s">
-        <v>195</v>
-      </c>
       <c r="D51" s="82" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E51">
         <v>12</v>
@@ -5563,13 +5560,13 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
+        <v>195</v>
+      </c>
+      <c r="C52" s="34" t="s">
         <v>196</v>
       </c>
-      <c r="C52" s="34" t="s">
+      <c r="D52" s="82" t="s">
         <v>197</v>
-      </c>
-      <c r="D52" s="82" t="s">
-        <v>198</v>
       </c>
       <c r="E52">
         <v>11</v>
@@ -5584,13 +5581,13 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
+        <v>198</v>
+      </c>
+      <c r="C53" s="34" t="s">
         <v>199</v>
       </c>
-      <c r="C53" s="34" t="s">
+      <c r="D53" s="82" t="s">
         <v>200</v>
-      </c>
-      <c r="D53" s="82" t="s">
-        <v>201</v>
       </c>
       <c r="E53">
         <v>10</v>
@@ -5605,13 +5602,13 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
+        <v>201</v>
+      </c>
+      <c r="C54" s="34" t="s">
         <v>202</v>
       </c>
-      <c r="C54" s="34" t="s">
+      <c r="D54" s="82" t="s">
         <v>203</v>
-      </c>
-      <c r="D54" s="82" t="s">
-        <v>204</v>
       </c>
       <c r="E54">
         <v>9</v>
@@ -5626,13 +5623,13 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
+        <v>204</v>
+      </c>
+      <c r="C55" s="34" t="s">
         <v>205</v>
       </c>
-      <c r="C55" s="34" t="s">
+      <c r="D55" s="82" t="s">
         <v>206</v>
-      </c>
-      <c r="D55" s="82" t="s">
-        <v>207</v>
       </c>
       <c r="E55">
         <v>8</v>
@@ -5647,13 +5644,13 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
+        <v>207</v>
+      </c>
+      <c r="C56" s="34" t="s">
         <v>208</v>
       </c>
-      <c r="C56" s="34" t="s">
+      <c r="D56" s="82" t="s">
         <v>209</v>
-      </c>
-      <c r="D56" s="82" t="s">
-        <v>210</v>
       </c>
       <c r="E56">
         <v>7</v>
@@ -5668,13 +5665,13 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
+        <v>210</v>
+      </c>
+      <c r="C57" s="34" t="s">
         <v>211</v>
       </c>
-      <c r="C57" s="34" t="s">
+      <c r="D57" s="82" t="s">
         <v>212</v>
-      </c>
-      <c r="D57" s="82" t="s">
-        <v>213</v>
       </c>
       <c r="E57">
         <v>6</v>
@@ -5689,13 +5686,13 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
+        <v>213</v>
+      </c>
+      <c r="C58" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="C58" s="34" t="s">
+      <c r="D58" s="82" t="s">
         <v>215</v>
-      </c>
-      <c r="D58" s="82" t="s">
-        <v>216</v>
       </c>
       <c r="E58">
         <v>5</v>
@@ -5710,13 +5707,13 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
+        <v>216</v>
+      </c>
+      <c r="C59" s="34" t="s">
         <v>217</v>
       </c>
-      <c r="C59" s="34" t="s">
+      <c r="D59" s="82" t="s">
         <v>218</v>
-      </c>
-      <c r="D59" s="82" t="s">
-        <v>219</v>
       </c>
       <c r="E59">
         <v>4</v>
@@ -5731,13 +5728,13 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
+        <v>219</v>
+      </c>
+      <c r="C60" s="34" t="s">
         <v>220</v>
       </c>
-      <c r="C60" s="34" t="s">
+      <c r="D60" s="82" t="s">
         <v>221</v>
-      </c>
-      <c r="D60" s="82" t="s">
-        <v>222</v>
       </c>
       <c r="E60">
         <v>3</v>
@@ -5752,13 +5749,13 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
+        <v>222</v>
+      </c>
+      <c r="C61" s="34" t="s">
         <v>223</v>
       </c>
-      <c r="C61" s="34" t="s">
-        <v>224</v>
-      </c>
       <c r="D61" s="82" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E61">
         <v>2</v>
@@ -5773,13 +5770,13 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
+        <v>224</v>
+      </c>
+      <c r="C62" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="C62" s="34" t="s">
+      <c r="D62" s="82" t="s">
         <v>226</v>
-      </c>
-      <c r="D62" s="82" t="s">
-        <v>227</v>
       </c>
       <c r="E62">
         <v>1</v>
@@ -5794,13 +5791,13 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C63" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="D63" s="82" t="s">
         <v>154</v>
-      </c>
-      <c r="D63" s="82" t="s">
-        <v>155</v>
       </c>
       <c r="E63">
         <v>1</v>
@@ -5815,13 +5812,13 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C64" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="D64" s="82" t="s">
         <v>156</v>
-      </c>
-      <c r="D64" s="82" t="s">
-        <v>157</v>
       </c>
       <c r="E64">
         <v>2</v>
@@ -5836,13 +5833,13 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C65" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="D65" s="82" t="s">
         <v>176</v>
-      </c>
-      <c r="D65" s="82" t="s">
-        <v>177</v>
       </c>
       <c r="E65">
         <v>99</v>
@@ -5857,13 +5854,13 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
+        <v>228</v>
+      </c>
+      <c r="C66" s="34" t="s">
         <v>229</v>
       </c>
-      <c r="C66" s="34" t="s">
-        <v>230</v>
-      </c>
       <c r="D66" s="82" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E66">
         <v>1</v>
@@ -5878,13 +5875,13 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
+        <v>230</v>
+      </c>
+      <c r="C67" s="34" t="s">
         <v>231</v>
       </c>
-      <c r="C67" s="34" t="s">
+      <c r="D67" s="82" t="s">
         <v>232</v>
-      </c>
-      <c r="D67" s="82" t="s">
-        <v>233</v>
       </c>
       <c r="E67">
         <v>1</v>
@@ -5899,13 +5896,13 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
+        <v>233</v>
+      </c>
+      <c r="C68" s="34" t="s">
         <v>234</v>
       </c>
-      <c r="C68" s="34" t="s">
+      <c r="D68" s="82" t="s">
         <v>235</v>
-      </c>
-      <c r="D68" s="82" t="s">
-        <v>236</v>
       </c>
       <c r="E68">
         <v>1</v>
@@ -5920,13 +5917,13 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
+        <v>236</v>
+      </c>
+      <c r="C69" s="34" t="s">
         <v>237</v>
       </c>
-      <c r="C69" s="34" t="s">
+      <c r="D69" s="82" t="s">
         <v>238</v>
-      </c>
-      <c r="D69" s="82" t="s">
-        <v>239</v>
       </c>
       <c r="E69">
         <v>1</v>
@@ -5941,13 +5938,13 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
+        <v>239</v>
+      </c>
+      <c r="C70" s="34" t="s">
         <v>240</v>
       </c>
-      <c r="C70" s="34" t="s">
+      <c r="D70" s="82" t="s">
         <v>241</v>
-      </c>
-      <c r="D70" s="82" t="s">
-        <v>242</v>
       </c>
       <c r="E70">
         <v>1</v>
@@ -5962,13 +5959,13 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
+        <v>242</v>
+      </c>
+      <c r="C71" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="C71" s="34" t="s">
+      <c r="D71" s="82" t="s">
         <v>244</v>
-      </c>
-      <c r="D71" s="82" t="s">
-        <v>245</v>
       </c>
       <c r="E71">
         <v>1</v>
@@ -5983,13 +5980,13 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
+        <v>245</v>
+      </c>
+      <c r="C72" s="34" t="s">
         <v>246</v>
       </c>
-      <c r="C72" s="34" t="s">
+      <c r="D72" s="82" t="s">
         <v>247</v>
-      </c>
-      <c r="D72" s="82" t="s">
-        <v>248</v>
       </c>
       <c r="E72">
         <v>1</v>
@@ -6004,13 +6001,13 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
+        <v>248</v>
+      </c>
+      <c r="C73" s="34" t="s">
         <v>249</v>
       </c>
-      <c r="C73" s="34" t="s">
+      <c r="D73" s="82" t="s">
         <v>250</v>
-      </c>
-      <c r="D73" s="82" t="s">
-        <v>251</v>
       </c>
       <c r="E73">
         <v>1</v>
@@ -6025,13 +6022,13 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
+        <v>251</v>
+      </c>
+      <c r="C74" s="34" t="s">
         <v>252</v>
       </c>
-      <c r="C74" s="34" t="s">
+      <c r="D74" s="82" t="s">
         <v>253</v>
-      </c>
-      <c r="D74" s="82" t="s">
-        <v>254</v>
       </c>
       <c r="E74">
         <v>1</v>
@@ -6046,13 +6043,13 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
+        <v>254</v>
+      </c>
+      <c r="C75" s="34" t="s">
         <v>255</v>
       </c>
-      <c r="C75" s="34" t="s">
+      <c r="D75" s="82" t="s">
         <v>256</v>
-      </c>
-      <c r="D75" s="82" t="s">
-        <v>257</v>
       </c>
       <c r="E75">
         <v>1</v>
@@ -6067,13 +6064,13 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
+        <v>257</v>
+      </c>
+      <c r="C76" s="34" t="s">
         <v>258</v>
       </c>
-      <c r="C76" s="34" t="s">
+      <c r="D76" s="82" t="s">
         <v>259</v>
-      </c>
-      <c r="D76" s="82" t="s">
-        <v>260</v>
       </c>
       <c r="E76">
         <v>1</v>
@@ -6088,13 +6085,13 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
+        <v>260</v>
+      </c>
+      <c r="C77" s="34" t="s">
         <v>261</v>
       </c>
-      <c r="C77" s="34" t="s">
+      <c r="D77" s="82" t="s">
         <v>262</v>
-      </c>
-      <c r="D77" s="82" t="s">
-        <v>263</v>
       </c>
       <c r="E77">
         <v>1</v>
@@ -6109,13 +6106,13 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
+        <v>263</v>
+      </c>
+      <c r="C78" s="34" t="s">
         <v>264</v>
       </c>
-      <c r="C78" s="34" t="s">
+      <c r="D78" s="82" t="s">
         <v>265</v>
-      </c>
-      <c r="D78" s="82" t="s">
-        <v>266</v>
       </c>
       <c r="E78">
         <v>1</v>
@@ -6130,13 +6127,13 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
+        <v>266</v>
+      </c>
+      <c r="C79" s="34" t="s">
         <v>267</v>
       </c>
-      <c r="C79" s="34" t="s">
+      <c r="D79" s="82" t="s">
         <v>268</v>
-      </c>
-      <c r="D79" s="82" t="s">
-        <v>269</v>
       </c>
       <c r="E79">
         <v>1</v>
@@ -6151,13 +6148,13 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
+        <v>269</v>
+      </c>
+      <c r="C80" s="34" t="s">
         <v>270</v>
       </c>
-      <c r="C80" s="34" t="s">
+      <c r="D80" s="82" t="s">
         <v>271</v>
-      </c>
-      <c r="D80" s="82" t="s">
-        <v>272</v>
       </c>
       <c r="E80">
         <v>1</v>
@@ -6172,13 +6169,13 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
+        <v>272</v>
+      </c>
+      <c r="C81" s="34" t="s">
         <v>273</v>
       </c>
-      <c r="C81" s="34" t="s">
+      <c r="D81" s="82" t="s">
         <v>274</v>
-      </c>
-      <c r="D81" s="82" t="s">
-        <v>275</v>
       </c>
       <c r="E81">
         <v>1</v>
@@ -6193,13 +6190,13 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
+        <v>275</v>
+      </c>
+      <c r="C82" s="34" t="s">
         <v>276</v>
       </c>
-      <c r="C82" s="34" t="s">
+      <c r="D82" s="82" t="s">
         <v>277</v>
-      </c>
-      <c r="D82" s="82" t="s">
-        <v>278</v>
       </c>
       <c r="E82">
         <v>1</v>
@@ -6214,13 +6211,13 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
+        <v>278</v>
+      </c>
+      <c r="C83" s="34" t="s">
         <v>279</v>
       </c>
-      <c r="C83" s="34" t="s">
+      <c r="D83" s="82" t="s">
         <v>280</v>
-      </c>
-      <c r="D83" s="82" t="s">
-        <v>281</v>
       </c>
       <c r="E83">
         <v>1</v>
@@ -6235,13 +6232,13 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
+        <v>281</v>
+      </c>
+      <c r="C84" s="34" t="s">
         <v>282</v>
       </c>
-      <c r="C84" s="34" t="s">
+      <c r="D84" s="82" t="s">
         <v>283</v>
-      </c>
-      <c r="D84" s="82" t="s">
-        <v>284</v>
       </c>
       <c r="E84">
         <v>1</v>
@@ -6256,19 +6253,19 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C85" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="D85" s="82" t="s">
         <v>154</v>
-      </c>
-      <c r="D85" s="82" t="s">
-        <v>155</v>
       </c>
       <c r="E85">
         <v>1</v>
       </c>
       <c r="F85" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H85" s="35" t="str">
         <f t="shared" si="1"/>
@@ -6280,13 +6277,13 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C86" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="D86" s="82" t="s">
         <v>156</v>
-      </c>
-      <c r="D86" s="82" t="s">
-        <v>157</v>
       </c>
       <c r="E86">
         <v>2</v>
@@ -6301,13 +6298,13 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
+        <v>284</v>
+      </c>
+      <c r="C87" s="34" t="s">
         <v>285</v>
       </c>
-      <c r="C87" s="34" t="s">
+      <c r="D87" s="82" t="s">
         <v>286</v>
-      </c>
-      <c r="D87" s="82" t="s">
-        <v>287</v>
       </c>
       <c r="E87">
         <v>14</v>
@@ -6322,13 +6319,13 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
+        <v>287</v>
+      </c>
+      <c r="C88" s="34" t="s">
         <v>288</v>
       </c>
-      <c r="C88" s="34" t="s">
+      <c r="D88" s="82" t="s">
         <v>289</v>
-      </c>
-      <c r="D88" s="82" t="s">
-        <v>290</v>
       </c>
       <c r="E88">
         <v>13</v>
@@ -6343,13 +6340,13 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
+        <v>290</v>
+      </c>
+      <c r="C89" s="34" t="s">
         <v>291</v>
       </c>
-      <c r="C89" s="34" t="s">
+      <c r="D89" s="82" t="s">
         <v>292</v>
-      </c>
-      <c r="D89" s="82" t="s">
-        <v>293</v>
       </c>
       <c r="E89">
         <v>12</v>
@@ -6364,13 +6361,13 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
+        <v>293</v>
+      </c>
+      <c r="C90" s="34" t="s">
         <v>294</v>
       </c>
-      <c r="C90" s="34" t="s">
+      <c r="D90" s="82" t="s">
         <v>295</v>
-      </c>
-      <c r="D90" s="82" t="s">
-        <v>296</v>
       </c>
       <c r="E90">
         <v>11</v>
@@ -6385,13 +6382,13 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
+        <v>296</v>
+      </c>
+      <c r="C91" s="34" t="s">
         <v>297</v>
       </c>
-      <c r="C91" s="34" t="s">
+      <c r="D91" s="82" t="s">
         <v>298</v>
-      </c>
-      <c r="D91" s="82" t="s">
-        <v>299</v>
       </c>
       <c r="E91">
         <v>10</v>
@@ -6406,13 +6403,13 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
+        <v>299</v>
+      </c>
+      <c r="C92" s="34" t="s">
         <v>300</v>
       </c>
-      <c r="C92" s="34" t="s">
-        <v>301</v>
-      </c>
       <c r="D92" s="82" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E92">
         <v>9</v>
@@ -6427,13 +6424,13 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
+        <v>301</v>
+      </c>
+      <c r="C93" s="34" t="s">
         <v>302</v>
       </c>
-      <c r="C93" s="34" t="s">
+      <c r="D93" s="82" t="s">
         <v>303</v>
-      </c>
-      <c r="D93" s="82" t="s">
-        <v>304</v>
       </c>
       <c r="E93">
         <v>8</v>
@@ -6448,13 +6445,13 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
+        <v>304</v>
+      </c>
+      <c r="C94" s="34" t="s">
         <v>305</v>
       </c>
-      <c r="C94" s="34" t="s">
-        <v>306</v>
-      </c>
       <c r="D94" s="82" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E94">
         <v>7</v>
@@ -6469,13 +6466,13 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
+        <v>306</v>
+      </c>
+      <c r="C95" s="34" t="s">
         <v>307</v>
       </c>
-      <c r="C95" s="34" t="s">
+      <c r="D95" s="82" t="s">
         <v>308</v>
-      </c>
-      <c r="D95" s="82" t="s">
-        <v>309</v>
       </c>
       <c r="E95">
         <v>6</v>
@@ -6490,13 +6487,13 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
+        <v>309</v>
+      </c>
+      <c r="C96" s="34" t="s">
         <v>310</v>
       </c>
-      <c r="C96" s="34" t="s">
+      <c r="D96" s="82" t="s">
         <v>311</v>
-      </c>
-      <c r="D96" s="82" t="s">
-        <v>312</v>
       </c>
       <c r="E96">
         <v>5</v>
@@ -6511,13 +6508,13 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
+        <v>312</v>
+      </c>
+      <c r="C97" s="34" t="s">
         <v>313</v>
       </c>
-      <c r="C97" s="34" t="s">
-        <v>314</v>
-      </c>
       <c r="D97" s="82" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E97">
         <v>4</v>
@@ -6532,13 +6529,13 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
+        <v>314</v>
+      </c>
+      <c r="C98" s="34" t="s">
         <v>315</v>
       </c>
-      <c r="C98" s="34" t="s">
+      <c r="D98" s="82" t="s">
         <v>316</v>
-      </c>
-      <c r="D98" s="82" t="s">
-        <v>317</v>
       </c>
       <c r="E98">
         <v>3</v>
@@ -6553,13 +6550,13 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
+        <v>317</v>
+      </c>
+      <c r="C99" s="34" t="s">
         <v>318</v>
       </c>
-      <c r="C99" s="34" t="s">
+      <c r="D99" s="82" t="s">
         <v>319</v>
-      </c>
-      <c r="D99" s="82" t="s">
-        <v>320</v>
       </c>
       <c r="E99">
         <v>2</v>
@@ -6574,13 +6571,13 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
+        <v>320</v>
+      </c>
+      <c r="C100" s="34" t="s">
         <v>321</v>
       </c>
-      <c r="C100" s="34" t="s">
-        <v>322</v>
-      </c>
       <c r="D100" s="82" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E100">
         <v>1</v>
@@ -6595,13 +6592,13 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
+        <v>322</v>
+      </c>
+      <c r="C101" s="34" t="s">
         <v>323</v>
       </c>
-      <c r="C101" s="34" t="s">
+      <c r="D101" s="82" t="s">
         <v>324</v>
-      </c>
-      <c r="D101" s="82" t="s">
-        <v>325</v>
       </c>
       <c r="E101">
         <v>1</v>
@@ -6616,13 +6613,13 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C102" s="34" t="s">
+        <v>325</v>
+      </c>
+      <c r="D102" s="82" t="s">
         <v>326</v>
-      </c>
-      <c r="D102" s="82" t="s">
-        <v>327</v>
       </c>
       <c r="E102">
         <v>66</v>
@@ -6637,13 +6634,13 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C103" s="34" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D103" s="82" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E103">
         <v>99</v>
@@ -6658,13 +6655,13 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C104" s="34" t="s">
+        <v>328</v>
+      </c>
+      <c r="D104" s="82" t="s">
         <v>329</v>
-      </c>
-      <c r="D104" s="82" t="s">
-        <v>330</v>
       </c>
       <c r="E104">
         <v>2</v>
@@ -6679,19 +6676,19 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C105" s="34" t="s">
+        <v>323</v>
+      </c>
+      <c r="D105" s="82" t="s">
         <v>324</v>
-      </c>
-      <c r="D105" s="82" t="s">
-        <v>325</v>
       </c>
       <c r="E105">
         <v>1</v>
       </c>
       <c r="F105" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H105" s="35" t="str">
         <f t="shared" si="1"/>
@@ -6703,13 +6700,13 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C106" s="34" t="s">
+        <v>325</v>
+      </c>
+      <c r="D106" s="82" t="s">
         <v>326</v>
-      </c>
-      <c r="D106" s="82" t="s">
-        <v>327</v>
       </c>
       <c r="E106">
         <v>66</v>
@@ -6724,13 +6721,13 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C107" s="34" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D107" s="82" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E107">
         <v>99</v>
@@ -6745,10 +6742,10 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C108" s="34" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D108" s="82" t="s">
         <v>56</v>
@@ -6757,7 +6754,7 @@
         <v>77</v>
       </c>
       <c r="F108" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="H108" s="35" t="str">
         <f t="shared" si="1"/>
@@ -6769,19 +6766,19 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C109" s="34" t="s">
+        <v>323</v>
+      </c>
+      <c r="D109" s="82" t="s">
         <v>324</v>
-      </c>
-      <c r="D109" s="82" t="s">
-        <v>325</v>
       </c>
       <c r="E109">
         <v>1</v>
       </c>
       <c r="F109" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H109" s="35" t="str">
         <f t="shared" si="1"/>
@@ -6793,13 +6790,13 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C110" s="34" t="s">
+        <v>325</v>
+      </c>
+      <c r="D110" s="82" t="s">
         <v>326</v>
-      </c>
-      <c r="D110" s="82" t="s">
-        <v>327</v>
       </c>
       <c r="E110">
         <v>66</v>
@@ -6814,13 +6811,13 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C111" s="34" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D111" s="82" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E111">
         <v>99</v>
@@ -6835,10 +6832,10 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C112" s="34" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D112" s="82" t="s">
         <v>56</v>
@@ -6847,7 +6844,7 @@
         <v>77</v>
       </c>
       <c r="F112" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="H112" s="35" t="str">
         <f t="shared" si="1"/>
@@ -6859,19 +6856,19 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C113" s="34" t="s">
+        <v>323</v>
+      </c>
+      <c r="D113" s="82" t="s">
         <v>324</v>
-      </c>
-      <c r="D113" s="82" t="s">
-        <v>325</v>
       </c>
       <c r="E113">
         <v>1</v>
       </c>
       <c r="F113" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H113" s="35" t="str">
         <f t="shared" si="1"/>
@@ -6883,13 +6880,13 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C114" s="34" t="s">
+        <v>325</v>
+      </c>
+      <c r="D114" s="82" t="s">
         <v>326</v>
-      </c>
-      <c r="D114" s="82" t="s">
-        <v>327</v>
       </c>
       <c r="E114">
         <v>66</v>
@@ -6904,13 +6901,13 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C115" s="34" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D115" s="82" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E115">
         <v>99</v>
@@ -6925,10 +6922,10 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C116" s="34" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D116" s="82" t="s">
         <v>56</v>
@@ -6937,7 +6934,7 @@
         <v>77</v>
       </c>
       <c r="F116" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H116" s="35" t="str">
         <f t="shared" si="1"/>
@@ -6949,19 +6946,19 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C117" s="34" t="s">
+        <v>323</v>
+      </c>
+      <c r="D117" s="82" t="s">
         <v>324</v>
-      </c>
-      <c r="D117" s="82" t="s">
-        <v>325</v>
       </c>
       <c r="E117">
         <v>1</v>
       </c>
       <c r="F117" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H117" s="35" t="str">
         <f t="shared" si="1"/>
@@ -6973,13 +6970,13 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C118" s="34" t="s">
+        <v>325</v>
+      </c>
+      <c r="D118" s="82" t="s">
         <v>326</v>
-      </c>
-      <c r="D118" s="82" t="s">
-        <v>327</v>
       </c>
       <c r="E118">
         <v>66</v>
@@ -6994,13 +6991,13 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C119" s="34" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D119" s="82" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E119">
         <v>99</v>
@@ -7015,10 +7012,10 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C120" s="34" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D120" s="82" t="s">
         <v>56</v>
@@ -7027,7 +7024,7 @@
         <v>77</v>
       </c>
       <c r="F120" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H120" s="35" t="str">
         <f t="shared" si="1"/>
@@ -7039,19 +7036,19 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C121" s="34" t="s">
+        <v>323</v>
+      </c>
+      <c r="D121" s="82" t="s">
         <v>324</v>
-      </c>
-      <c r="D121" s="82" t="s">
-        <v>325</v>
       </c>
       <c r="E121">
         <v>1</v>
       </c>
       <c r="F121" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H121" s="35" t="str">
         <f t="shared" si="1"/>
@@ -7063,13 +7060,13 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C122" s="34" t="s">
+        <v>325</v>
+      </c>
+      <c r="D122" s="82" t="s">
         <v>326</v>
-      </c>
-      <c r="D122" s="82" t="s">
-        <v>327</v>
       </c>
       <c r="E122">
         <v>66</v>
@@ -7084,13 +7081,13 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C123" s="34" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D123" s="82" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E123">
         <v>99</v>
@@ -7105,19 +7102,19 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C124" s="34" t="s">
+        <v>342</v>
+      </c>
+      <c r="D124" s="82" t="s">
         <v>343</v>
-      </c>
-      <c r="D124" s="82" t="s">
-        <v>344</v>
       </c>
       <c r="E124">
         <v>1</v>
       </c>
       <c r="F124" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H124" s="35" t="str">
         <f t="shared" si="1"/>
@@ -7129,13 +7126,13 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C125" s="34" t="s">
+        <v>325</v>
+      </c>
+      <c r="D125" s="82" t="s">
         <v>326</v>
-      </c>
-      <c r="D125" s="82" t="s">
-        <v>327</v>
       </c>
       <c r="E125">
         <v>66</v>
@@ -7150,19 +7147,19 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C126" s="34" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D126" s="82" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E126">
         <v>99</v>
       </c>
       <c r="F126" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H126" s="35" t="str">
         <f t="shared" si="1"/>
@@ -7174,19 +7171,19 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C127" s="34" t="s">
+        <v>328</v>
+      </c>
+      <c r="D127" s="82" t="s">
         <v>329</v>
-      </c>
-      <c r="D127" s="82" t="s">
-        <v>330</v>
       </c>
       <c r="E127">
         <v>2</v>
       </c>
       <c r="F127" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H127" s="35" t="str">
         <f t="shared" si="1"/>
@@ -7198,13 +7195,13 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C128" s="34" t="s">
+        <v>344</v>
+      </c>
+      <c r="D128" s="82" t="s">
         <v>345</v>
-      </c>
-      <c r="D128" s="82" t="s">
-        <v>346</v>
       </c>
       <c r="E128">
         <v>1</v>
@@ -7219,13 +7216,13 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C129" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="D129" s="82" t="s">
         <v>347</v>
-      </c>
-      <c r="D129" s="82" t="s">
-        <v>348</v>
       </c>
       <c r="E129">
         <v>2</v>
@@ -7240,13 +7237,13 @@
         <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C130" s="34" t="s">
+        <v>348</v>
+      </c>
+      <c r="D130" s="82" t="s">
         <v>349</v>
-      </c>
-      <c r="D130" s="82" t="s">
-        <v>350</v>
       </c>
       <c r="E130">
         <v>3</v>
@@ -7261,13 +7258,13 @@
         <v>130</v>
       </c>
       <c r="B131" t="s">
+        <v>350</v>
+      </c>
+      <c r="C131" s="34" t="s">
         <v>351</v>
       </c>
-      <c r="C131" s="34" t="s">
+      <c r="D131" s="82" t="s">
         <v>352</v>
-      </c>
-      <c r="D131" s="82" t="s">
-        <v>353</v>
       </c>
       <c r="E131">
         <v>4</v>
@@ -7282,13 +7279,13 @@
         <v>131</v>
       </c>
       <c r="B132" t="s">
+        <v>353</v>
+      </c>
+      <c r="C132" s="34" t="s">
         <v>354</v>
       </c>
-      <c r="C132" s="34" t="s">
+      <c r="D132" s="82" t="s">
         <v>355</v>
-      </c>
-      <c r="D132" s="82" t="s">
-        <v>356</v>
       </c>
       <c r="E132">
         <v>3</v>
@@ -7303,13 +7300,13 @@
         <v>132</v>
       </c>
       <c r="B133" t="s">
+        <v>356</v>
+      </c>
+      <c r="C133" s="34" t="s">
         <v>357</v>
       </c>
-      <c r="C133" s="34" t="s">
+      <c r="D133" s="82" t="s">
         <v>358</v>
-      </c>
-      <c r="D133" s="82" t="s">
-        <v>359</v>
       </c>
       <c r="E133">
         <v>2</v>
@@ -7324,13 +7321,13 @@
         <v>133</v>
       </c>
       <c r="B134" t="s">
+        <v>359</v>
+      </c>
+      <c r="C134" s="34" t="s">
         <v>360</v>
       </c>
-      <c r="C134" s="34" t="s">
+      <c r="D134" s="82" t="s">
         <v>361</v>
-      </c>
-      <c r="D134" s="82" t="s">
-        <v>362</v>
       </c>
       <c r="E134">
         <v>1</v>
@@ -7345,13 +7342,13 @@
         <v>134</v>
       </c>
       <c r="B135" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C135" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="D135" s="82" t="s">
         <v>154</v>
-      </c>
-      <c r="D135" s="82" t="s">
-        <v>155</v>
       </c>
       <c r="E135">
         <v>1</v>
@@ -7366,13 +7363,13 @@
         <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C136" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="D136" s="82" t="s">
         <v>156</v>
-      </c>
-      <c r="D136" s="82" t="s">
-        <v>157</v>
       </c>
       <c r="E136">
         <v>2</v>
@@ -7387,13 +7384,13 @@
         <v>136</v>
       </c>
       <c r="B137" t="s">
+        <v>364</v>
+      </c>
+      <c r="C137" s="34" t="s">
         <v>365</v>
       </c>
-      <c r="C137" s="34" t="s">
+      <c r="D137" s="82" t="s">
         <v>366</v>
-      </c>
-      <c r="D137" s="82" t="s">
-        <v>367</v>
       </c>
       <c r="E137">
         <v>99</v>
@@ -7408,13 +7405,13 @@
         <v>137</v>
       </c>
       <c r="B138" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C138" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="D138" s="82" t="s">
         <v>154</v>
-      </c>
-      <c r="D138" s="82" t="s">
-        <v>155</v>
       </c>
       <c r="E138">
         <v>1</v>
@@ -7429,13 +7426,13 @@
         <v>138</v>
       </c>
       <c r="B139" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C139" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="D139" s="82" t="s">
         <v>156</v>
-      </c>
-      <c r="D139" s="82" t="s">
-        <v>157</v>
       </c>
       <c r="E139">
         <v>2</v>

</xml_diff>

<commit_message>
some works done  for microbiome
</commit_message>
<xml_diff>
--- a/WBFFQ/DB and Documents/WBFFQ.xlsx
+++ b/WBFFQ/DB and Documents/WBFFQ.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-450" windowWidth="13485" windowHeight="12690"/>
+    <workbookView xWindow="-120" yWindow="-450" windowWidth="13485" windowHeight="12690" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="tbFormMain" sheetId="5" r:id="rId1"/>
@@ -1034,9 +1034,6 @@
     <t>c611_1</t>
   </si>
   <si>
-    <t>Khichuri (tick ‘yes’ and ask for the ingredients and code below according to food group),rice,bread?</t>
-  </si>
-  <si>
     <t>c611_Options_1</t>
   </si>
   <si>
@@ -1304,43 +1301,6 @@
   </si>
   <si>
     <r>
-      <t>w</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="SutonnyMJ"/>
-      </rPr>
-      <t xml:space="preserve">LPzox </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="SutonnyMJ"/>
-      </rPr>
-      <t xml:space="preserve">( </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="SutonnyMJ"/>
-      </rPr>
-      <t>w</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="SutonnyMJ"/>
-      </rPr>
-      <t>LPzox wK wK w`‡q ivbœv n‡q‡Q †R‡b wb‡q dzW MÖyc Abyhvqx bx‡P †KvW Kiyb),      fvZ,       iywU?</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>†L‡q‡Q wK Lvqwb</t>
     </r>
     <r>
@@ -1362,6 +1322,12 @@
   </si>
   <si>
     <t>FrmComboBox</t>
+  </si>
+  <si>
+    <t>wLPzox ,fvZ,iywU?</t>
+  </si>
+  <si>
+    <t>Khichuri, rice, bread?</t>
   </si>
 </sst>
 </file>
@@ -1668,7 +1634,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1898,6 +1864,9 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="46">
@@ -2240,8 +2209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:DK67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="T24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="U2" sqref="U2:U31"/>
@@ -2585,7 +2554,7 @@
       </c>
       <c r="G5" s="66"/>
       <c r="H5" s="65" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="I5" s="58"/>
       <c r="J5" s="62"/>
@@ -2615,7 +2584,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="65" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C6" s="58" t="s">
         <v>26</v>
@@ -2627,11 +2596,11 @@
         <v>1.8</v>
       </c>
       <c r="F6" s="68" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G6" s="66"/>
       <c r="H6" s="65" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="I6" s="58"/>
       <c r="L6" s="63"/>
@@ -2659,7 +2628,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="65" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C7" s="58" t="s">
         <v>23</v>
@@ -2671,11 +2640,11 @@
         <v>1.9</v>
       </c>
       <c r="F7" s="68" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G7" s="66"/>
       <c r="H7" s="65" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="I7" s="58"/>
       <c r="L7" s="63"/>
@@ -2703,10 +2672,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="65" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C8" s="58" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D8" s="58" t="s">
         <v>27</v>
@@ -2715,7 +2684,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="F8" s="68" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G8" s="66"/>
       <c r="H8" s="65" t="s">
@@ -4441,7 +4410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H140"/>
   <sheetViews>
-    <sheetView topLeftCell="A123" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H2" sqref="H2:H139"/>
     </sheetView>
   </sheetViews>
@@ -5428,7 +5397,7 @@
         <v>191</v>
       </c>
       <c r="D46" s="82" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E46">
         <v>6</v>
@@ -5545,7 +5514,7 @@
         <v>194</v>
       </c>
       <c r="D51" s="82" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E51">
         <v>12</v>
@@ -5860,7 +5829,7 @@
         <v>229</v>
       </c>
       <c r="D66" s="82" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E66">
         <v>1</v>
@@ -6409,7 +6378,7 @@
         <v>300</v>
       </c>
       <c r="D92" s="82" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E92">
         <v>9</v>
@@ -6451,7 +6420,7 @@
         <v>305</v>
       </c>
       <c r="D94" s="82" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E94">
         <v>7</v>
@@ -6514,7 +6483,7 @@
         <v>313</v>
       </c>
       <c r="D97" s="82" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E97">
         <v>4</v>
@@ -6566,7 +6535,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('98','c611_2', 'Pumpkin, carrots?','wgwó Kzgov, MvRi?','2','');</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="66">
+    <row r="100" spans="1:8" ht="16.5">
       <c r="A100" s="35">
         <v>99</v>
       </c>
@@ -6574,17 +6543,17 @@
         <v>320</v>
       </c>
       <c r="C100" s="34" t="s">
-        <v>321</v>
-      </c>
-      <c r="D100" s="82" t="s">
-        <v>379</v>
+        <v>381</v>
+      </c>
+      <c r="D100" s="88" t="s">
+        <v>380</v>
       </c>
       <c r="E100">
         <v>1</v>
       </c>
       <c r="H100" s="35" t="str">
         <f t="shared" si="1"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('99','c611_1', 'Khichuri (tick ‘yes’ and ask for the ingredients and code below according to food group),rice,bread?','wLPzox ( wLPzox wK wK w`‡q ivbœv n‡q‡Q †R‡b wb‡q dzW MÖyc Abyhvqx bx‡P †KvW Kiyb),      fvZ,       iywU?','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('99','c611_1', 'Khichuri, rice, bread?','wLPzox ,fvZ,iywU?','1','');</v>
       </c>
     </row>
     <row r="101" spans="1:8">
@@ -6592,13 +6561,13 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
+        <v>321</v>
+      </c>
+      <c r="C101" s="34" t="s">
         <v>322</v>
       </c>
-      <c r="C101" s="34" t="s">
+      <c r="D101" s="82" t="s">
         <v>323</v>
-      </c>
-      <c r="D101" s="82" t="s">
-        <v>324</v>
       </c>
       <c r="E101">
         <v>1</v>
@@ -6613,13 +6582,13 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C102" s="34" t="s">
+        <v>324</v>
+      </c>
+      <c r="D102" s="82" t="s">
         <v>325</v>
-      </c>
-      <c r="D102" s="82" t="s">
-        <v>326</v>
       </c>
       <c r="E102">
         <v>66</v>
@@ -6634,13 +6603,13 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C103" s="34" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D103" s="82" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E103">
         <v>99</v>
@@ -6655,13 +6624,13 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C104" s="34" t="s">
+        <v>327</v>
+      </c>
+      <c r="D104" s="82" t="s">
         <v>328</v>
-      </c>
-      <c r="D104" s="82" t="s">
-        <v>329</v>
       </c>
       <c r="E104">
         <v>2</v>
@@ -6679,16 +6648,16 @@
         <v>91</v>
       </c>
       <c r="C105" s="34" t="s">
+        <v>322</v>
+      </c>
+      <c r="D105" s="82" t="s">
         <v>323</v>
-      </c>
-      <c r="D105" s="82" t="s">
-        <v>324</v>
       </c>
       <c r="E105">
         <v>1</v>
       </c>
       <c r="F105" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="H105" s="35" t="str">
         <f t="shared" si="1"/>
@@ -6703,10 +6672,10 @@
         <v>91</v>
       </c>
       <c r="C106" s="34" t="s">
+        <v>324</v>
+      </c>
+      <c r="D106" s="82" t="s">
         <v>325</v>
-      </c>
-      <c r="D106" s="82" t="s">
-        <v>326</v>
       </c>
       <c r="E106">
         <v>66</v>
@@ -6724,10 +6693,10 @@
         <v>91</v>
       </c>
       <c r="C107" s="34" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D107" s="82" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E107">
         <v>99</v>
@@ -6754,7 +6723,7 @@
         <v>77</v>
       </c>
       <c r="F108" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H108" s="35" t="str">
         <f t="shared" si="1"/>
@@ -6766,19 +6735,19 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C109" s="34" t="s">
+        <v>322</v>
+      </c>
+      <c r="D109" s="82" t="s">
         <v>323</v>
-      </c>
-      <c r="D109" s="82" t="s">
-        <v>324</v>
       </c>
       <c r="E109">
         <v>1</v>
       </c>
       <c r="F109" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H109" s="35" t="str">
         <f t="shared" si="1"/>
@@ -6790,13 +6759,13 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C110" s="34" t="s">
+        <v>324</v>
+      </c>
+      <c r="D110" s="82" t="s">
         <v>325</v>
-      </c>
-      <c r="D110" s="82" t="s">
-        <v>326</v>
       </c>
       <c r="E110">
         <v>66</v>
@@ -6811,13 +6780,13 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C111" s="34" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D111" s="82" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E111">
         <v>99</v>
@@ -6832,7 +6801,7 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C112" s="34" t="s">
         <v>192</v>
@@ -6844,7 +6813,7 @@
         <v>77</v>
       </c>
       <c r="F112" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H112" s="35" t="str">
         <f t="shared" si="1"/>
@@ -6856,19 +6825,19 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C113" s="34" t="s">
+        <v>322</v>
+      </c>
+      <c r="D113" s="82" t="s">
         <v>323</v>
-      </c>
-      <c r="D113" s="82" t="s">
-        <v>324</v>
       </c>
       <c r="E113">
         <v>1</v>
       </c>
       <c r="F113" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H113" s="35" t="str">
         <f t="shared" si="1"/>
@@ -6880,13 +6849,13 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C114" s="34" t="s">
+        <v>324</v>
+      </c>
+      <c r="D114" s="82" t="s">
         <v>325</v>
-      </c>
-      <c r="D114" s="82" t="s">
-        <v>326</v>
       </c>
       <c r="E114">
         <v>66</v>
@@ -6901,13 +6870,13 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C115" s="34" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D115" s="82" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E115">
         <v>99</v>
@@ -6922,7 +6891,7 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C116" s="34" t="s">
         <v>192</v>
@@ -6934,7 +6903,7 @@
         <v>77</v>
       </c>
       <c r="F116" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H116" s="35" t="str">
         <f t="shared" si="1"/>
@@ -6946,19 +6915,19 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C117" s="34" t="s">
+        <v>322</v>
+      </c>
+      <c r="D117" s="82" t="s">
         <v>323</v>
-      </c>
-      <c r="D117" s="82" t="s">
-        <v>324</v>
       </c>
       <c r="E117">
         <v>1</v>
       </c>
       <c r="F117" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H117" s="35" t="str">
         <f t="shared" si="1"/>
@@ -6970,13 +6939,13 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C118" s="34" t="s">
+        <v>324</v>
+      </c>
+      <c r="D118" s="82" t="s">
         <v>325</v>
-      </c>
-      <c r="D118" s="82" t="s">
-        <v>326</v>
       </c>
       <c r="E118">
         <v>66</v>
@@ -6991,13 +6960,13 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C119" s="34" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D119" s="82" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E119">
         <v>99</v>
@@ -7012,7 +6981,7 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C120" s="34" t="s">
         <v>192</v>
@@ -7024,7 +6993,7 @@
         <v>77</v>
       </c>
       <c r="F120" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H120" s="35" t="str">
         <f t="shared" si="1"/>
@@ -7036,19 +7005,19 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C121" s="34" t="s">
+        <v>322</v>
+      </c>
+      <c r="D121" s="82" t="s">
         <v>323</v>
-      </c>
-      <c r="D121" s="82" t="s">
-        <v>324</v>
       </c>
       <c r="E121">
         <v>1</v>
       </c>
       <c r="F121" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="H121" s="35" t="str">
         <f t="shared" si="1"/>
@@ -7060,13 +7029,13 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C122" s="34" t="s">
+        <v>324</v>
+      </c>
+      <c r="D122" s="82" t="s">
         <v>325</v>
-      </c>
-      <c r="D122" s="82" t="s">
-        <v>326</v>
       </c>
       <c r="E122">
         <v>66</v>
@@ -7081,13 +7050,13 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C123" s="34" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D123" s="82" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E123">
         <v>99</v>
@@ -7105,10 +7074,10 @@
         <v>86</v>
       </c>
       <c r="C124" s="34" t="s">
+        <v>341</v>
+      </c>
+      <c r="D124" s="82" t="s">
         <v>342</v>
-      </c>
-      <c r="D124" s="82" t="s">
-        <v>343</v>
       </c>
       <c r="E124">
         <v>1</v>
@@ -7129,10 +7098,10 @@
         <v>86</v>
       </c>
       <c r="C125" s="34" t="s">
+        <v>324</v>
+      </c>
+      <c r="D125" s="82" t="s">
         <v>325</v>
-      </c>
-      <c r="D125" s="82" t="s">
-        <v>326</v>
       </c>
       <c r="E125">
         <v>66</v>
@@ -7150,10 +7119,10 @@
         <v>86</v>
       </c>
       <c r="C126" s="34" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D126" s="82" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E126">
         <v>99</v>
@@ -7174,10 +7143,10 @@
         <v>86</v>
       </c>
       <c r="C127" s="34" t="s">
+        <v>327</v>
+      </c>
+      <c r="D127" s="82" t="s">
         <v>328</v>
-      </c>
-      <c r="D127" s="82" t="s">
-        <v>329</v>
       </c>
       <c r="E127">
         <v>2</v>
@@ -7198,10 +7167,10 @@
         <v>85</v>
       </c>
       <c r="C128" s="34" t="s">
+        <v>343</v>
+      </c>
+      <c r="D128" s="82" t="s">
         <v>344</v>
-      </c>
-      <c r="D128" s="82" t="s">
-        <v>345</v>
       </c>
       <c r="E128">
         <v>1</v>
@@ -7219,10 +7188,10 @@
         <v>85</v>
       </c>
       <c r="C129" s="34" t="s">
+        <v>345</v>
+      </c>
+      <c r="D129" s="82" t="s">
         <v>346</v>
-      </c>
-      <c r="D129" s="82" t="s">
-        <v>347</v>
       </c>
       <c r="E129">
         <v>2</v>
@@ -7240,10 +7209,10 @@
         <v>85</v>
       </c>
       <c r="C130" s="34" t="s">
+        <v>347</v>
+      </c>
+      <c r="D130" s="82" t="s">
         <v>348</v>
-      </c>
-      <c r="D130" s="82" t="s">
-        <v>349</v>
       </c>
       <c r="E130">
         <v>3</v>
@@ -7258,13 +7227,13 @@
         <v>130</v>
       </c>
       <c r="B131" t="s">
+        <v>349</v>
+      </c>
+      <c r="C131" s="34" t="s">
         <v>350</v>
       </c>
-      <c r="C131" s="34" t="s">
+      <c r="D131" s="82" t="s">
         <v>351</v>
-      </c>
-      <c r="D131" s="82" t="s">
-        <v>352</v>
       </c>
       <c r="E131">
         <v>4</v>
@@ -7279,13 +7248,13 @@
         <v>131</v>
       </c>
       <c r="B132" t="s">
+        <v>352</v>
+      </c>
+      <c r="C132" s="34" t="s">
         <v>353</v>
       </c>
-      <c r="C132" s="34" t="s">
+      <c r="D132" s="82" t="s">
         <v>354</v>
-      </c>
-      <c r="D132" s="82" t="s">
-        <v>355</v>
       </c>
       <c r="E132">
         <v>3</v>
@@ -7300,13 +7269,13 @@
         <v>132</v>
       </c>
       <c r="B133" t="s">
+        <v>355</v>
+      </c>
+      <c r="C133" s="34" t="s">
         <v>356</v>
       </c>
-      <c r="C133" s="34" t="s">
+      <c r="D133" s="82" t="s">
         <v>357</v>
-      </c>
-      <c r="D133" s="82" t="s">
-        <v>358</v>
       </c>
       <c r="E133">
         <v>2</v>
@@ -7321,13 +7290,13 @@
         <v>133</v>
       </c>
       <c r="B134" t="s">
+        <v>358</v>
+      </c>
+      <c r="C134" s="34" t="s">
         <v>359</v>
       </c>
-      <c r="C134" s="34" t="s">
+      <c r="D134" s="82" t="s">
         <v>360</v>
-      </c>
-      <c r="D134" s="82" t="s">
-        <v>361</v>
       </c>
       <c r="E134">
         <v>1</v>
@@ -7342,7 +7311,7 @@
         <v>134</v>
       </c>
       <c r="B135" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C135" s="34" t="s">
         <v>153</v>
@@ -7363,7 +7332,7 @@
         <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C136" s="34" t="s">
         <v>155</v>
@@ -7384,13 +7353,13 @@
         <v>136</v>
       </c>
       <c r="B137" t="s">
+        <v>363</v>
+      </c>
+      <c r="C137" s="34" t="s">
         <v>364</v>
       </c>
-      <c r="C137" s="34" t="s">
+      <c r="D137" s="82" t="s">
         <v>365</v>
-      </c>
-      <c r="D137" s="82" t="s">
-        <v>366</v>
       </c>
       <c r="E137">
         <v>99</v>

</xml_diff>

<commit_message>
on 2nd june 2015
</commit_message>
<xml_diff>
--- a/WBFFQ/DB and Documents/WBFFQ.xlsx
+++ b/WBFFQ/DB and Documents/WBFFQ.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-450" windowWidth="13485" windowHeight="12690" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-450" windowWidth="13485" windowHeight="12690"/>
   </bookViews>
   <sheets>
     <sheet name="tbFormMain" sheetId="5" r:id="rId1"/>
@@ -2209,11 +2209,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:DK67"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="T26" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U2" sqref="U2:U31"/>
+      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="29.25" customHeight="1"/>
@@ -3033,7 +3033,7 @@
         <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('14', 'c603_other','FrmText', 'tblMainques','Ab¨vb¨ (wbwÏ©ó Kiyb)','Other (specify)','','M11','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
-    <row r="16" spans="1:115" s="12" customFormat="1" ht="19.5">
+    <row r="16" spans="1:115" s="12" customFormat="1" ht="25.5">
       <c r="A16" s="78">
         <v>15</v>
       </c>
@@ -4410,7 +4410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+    <sheetView topLeftCell="A47" workbookViewId="0">
       <selection activeCell="B104" sqref="B104"/>
     </sheetView>
   </sheetViews>

</xml_diff>